<commit_message>
Micropython setup, code not functional yet
</commit_message>
<xml_diff>
--- a/PartsList.xlsx
+++ b/PartsList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SuperYardage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CBE611-37D7-46D6-BE1D-A1F1BEBED0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CC7827-732E-4AA3-B99A-6B586F6D6579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -202,10 +202,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -490,7 +491,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -501,17 +502,17 @@
     <col min="4" max="4" width="46.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -522,7 +523,7 @@
       <c r="B2">
         <v>3400</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>37</v>
       </c>
       <c r="D2" t="s">
@@ -536,7 +537,7 @@
       <c r="B3">
         <v>1944</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
@@ -550,7 +551,7 @@
       <c r="B4">
         <v>3104</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
@@ -564,7 +565,7 @@
       <c r="B5">
         <v>1009</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
@@ -578,7 +579,7 @@
       <c r="B6">
         <v>5628</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
@@ -592,7 +593,7 @@
       <c r="B7">
         <v>5394</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
@@ -606,7 +607,7 @@
       <c r="B8">
         <v>258</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
@@ -620,7 +621,7 @@
       <c r="B9">
         <v>2011</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
@@ -634,7 +635,7 @@
       <c r="B10">
         <v>4422</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
@@ -648,7 +649,7 @@
       <c r="B11">
         <v>169</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
@@ -662,7 +663,7 @@
       <c r="B12">
         <v>807</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D12" t="s">
@@ -676,7 +677,7 @@
       <c r="B13">
         <v>160</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D13" t="s">
@@ -686,9 +687,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1" xr:uid="{64373DDE-46E8-43C3-A182-734F6615D0FF}"/>
-    <hyperlink ref="C2:C13" r:id="rId2" display="https://www.adafruit.com/product/3400" xr:uid="{E5121E5B-64D0-4AC3-BDA0-37A30097DA7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code for displaying cpu temp to tft display, pcb changes
</commit_message>
<xml_diff>
--- a/PartsList.xlsx
+++ b/PartsList.xlsx
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SuperYardage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CC7827-732E-4AA3-B99A-6B586F6D6579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315705BE-057A-4519-90D9-A94EE15F5026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Used" sheetId="1" r:id="rId1"/>
+    <sheet name="To Order" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -145,13 +157,85 @@
   </si>
   <si>
     <t>Microcomputer, Pi Zero 2 W also works</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/395</t>
+  </si>
+  <si>
+    <t>Level shifter</t>
+  </si>
+  <si>
+    <t>3.3 / 5 V logic converter</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/1956</t>
+  </si>
+  <si>
+    <t>Jumper wires</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/1008</t>
+  </si>
+  <si>
+    <t>alligator clips</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/153</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3165</t>
+  </si>
+  <si>
+    <t>wire</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/239</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3882</t>
+  </si>
+  <si>
+    <t>The Motor</t>
+  </si>
+  <si>
+    <t>My brother found this motor in one of his cd players so I decided to use it for this.  Turns out adafruit sells the same exact ones.  Not the best for this application but whatever</t>
+  </si>
+  <si>
+    <t>Breadboard</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/5682</t>
+  </si>
+  <si>
+    <t>Crimper</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/350</t>
+  </si>
+  <si>
+    <t>other crimper</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/147</t>
+  </si>
+  <si>
+    <t>wire strippers</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/527</t>
+  </si>
+  <si>
+    <t>more expensive wire strippers</t>
+  </si>
+  <si>
+    <t>other jumper wires</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +254,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,11 +293,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -488,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -684,6 +777,20 @@
         <v>32</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14">
+        <v>3882</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1" xr:uid="{64373DDE-46E8-43C3-A182-734F6615D0FF}"/>
@@ -691,4 +798,184 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8E06D9-D845-4BF7-A5C1-C992F6C87A45}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="33.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>395</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="5" t="str">
+        <f>HYPERLINK(A2)</f>
+        <v>Level shifter</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>1956</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <f t="shared" ref="D3:D11" si="0">HYPERLINK(A3)</f>
+        <v>Jumper wires</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>1008</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>alligator clips</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5">
+        <v>153</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>other jumper wires</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>3165</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>wire</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>239</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Breadboard</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Crimper</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>other crimper</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>wire strippers</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>more expensive wire strippers</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>